<commit_message>
updated tester code for utf encoding and updated testing stats
</commit_message>
<xml_diff>
--- a/Testing Statistics.xlsx
+++ b/Testing Statistics.xlsx
@@ -386,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -442,6 +442,26 @@
         <v>0.96799999999999997</v>
       </c>
     </row>
+    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B3" s="3">
+        <v>44286</v>
+      </c>
+      <c r="C3" s="2">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2">
+        <v>4</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.96799999999999997</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>

</xml_diff>

<commit_message>
testing stats and updated titlecase added
</commit_message>
<xml_diff>
--- a/Testing Statistics.xlsx
+++ b/Testing Statistics.xlsx
@@ -92,7 +92,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -104,6 +104,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -386,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F7" sqref="F7:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -482,6 +485,26 @@
         <v>0.97899999999999998</v>
       </c>
     </row>
+    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B5" s="3">
+        <v>44288</v>
+      </c>
+      <c r="C5" s="2">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2">
+        <v>34</v>
+      </c>
+      <c r="E5" s="2">
+        <v>4</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.94</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>

</xml_diff>